<commit_message>
decode unit stage 1
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\Misc\NIHIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D732A913-648B-432B-B049-3BB85B72D744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D25D934-445B-47E0-89FA-A9A2AE088C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25500" windowHeight="16605" xr2:uid="{AC58EBCB-9B6B-47F8-B1F9-E05E7C310A87}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="17385" xr2:uid="{AC58EBCB-9B6B-47F8-B1F9-E05E7C310A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="ALU" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="301">
   <si>
     <t>n0</t>
   </si>
@@ -996,14 +995,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="6">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1029,11 +1028,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1054,56 +1053,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1417,11 +1366,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA289FB-DB7B-4A58-B8AB-79807A2863A9}">
-  <dimension ref="A1:S134"/>
+  <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4325,82 +4274,25 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D127" s="3"/>
-      <c r="E127" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>279</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D128" s="3"/>
-      <c r="E128" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="H128" s="1" t="s">
-        <v>280</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D129" s="3"/>
-      <c r="E129" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="H129" s="1" t="s">
-        <v>284</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>99</v>
@@ -4413,71 +4305,143 @@
         <v>294</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D131" s="3"/>
+      <c r="E131" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D133" s="3"/>
+      <c r="E133" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C130:D130"/>
     <mergeCell ref="C96:D96"/>
     <mergeCell ref="C97:D97"/>
     <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I78 I119 E1:F9 I123:I124 E12:F99 G111:G126 E102:F1048576">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+  <conditionalFormatting sqref="I78 I119 E1:F9 I123:I124 E12:F99 G111:G126 E102:F126 E140:F1048576 E130:F137">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I111 I78">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="E1:E126 E140:E1048576 E130:E137">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Maybe"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4493,7 +4457,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4832,10 +4796,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added ROM addresses to spreadsheet
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\Misc\NIHIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D25D934-445B-47E0-89FA-A9A2AE088C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7F1638-CF1A-4E36-AB57-4699C44F516D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="17385" xr2:uid="{AC58EBCB-9B6B-47F8-B1F9-E05E7C310A87}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="17385" xr2:uid="{AC58EBCB-9B6B-47F8-B1F9-E05E7C310A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="308">
   <si>
     <t>n0</t>
   </si>
@@ -235,9 +235,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>mov R #</t>
-  </si>
-  <si>
     <t>Load immediate</t>
   </si>
   <si>
@@ -346,12 +343,6 @@
     <t>in P A R</t>
   </si>
   <si>
-    <t>output R to port P address A</t>
-  </si>
-  <si>
-    <t>input port P address A to R</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -883,15 +874,6 @@
     <t>Cache write</t>
   </si>
   <si>
-    <t>CRD R A</t>
-  </si>
-  <si>
-    <t>CWR R A</t>
-  </si>
-  <si>
-    <t>CRD H A</t>
-  </si>
-  <si>
     <t>16-bit cache read</t>
   </si>
   <si>
@@ -901,12 +883,6 @@
     <t>Maybe</t>
   </si>
   <si>
-    <t>CDL</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
     <t>Load Cache at RAM address A</t>
   </si>
   <si>
@@ -941,6 +917,51 @@
   </si>
   <si>
     <t>Short the capacitors</t>
+  </si>
+  <si>
+    <t>ROM Address</t>
+  </si>
+  <si>
+    <t>64;65;66;67</t>
+  </si>
+  <si>
+    <t>96;97</t>
+  </si>
+  <si>
+    <t>CDL #8</t>
+  </si>
+  <si>
+    <t>CST #8</t>
+  </si>
+  <si>
+    <t>mov R #8</t>
+  </si>
+  <si>
+    <t>CRD R #A</t>
+  </si>
+  <si>
+    <t>CWR R #A</t>
+  </si>
+  <si>
+    <t>CRD H #A</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>output R to port P address L</t>
+  </si>
+  <si>
+    <t>input port P address L to R</t>
+  </si>
+  <si>
+    <t>bits</t>
+  </si>
+  <si>
+    <t>stc</t>
+  </si>
+  <si>
+    <t>Set carry flag</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -991,11 +1012,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1369,8 +1403,8 @@
   <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,10 +1414,11 @@
     <col min="5" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1400,19 +1435,22 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1429,7 +1467,7 @@
         <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -1437,8 +1475,11 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1455,7 +1496,7 @@
         <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>32</v>
@@ -1463,8 +1504,11 @@
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1481,16 +1525,19 @@
         <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1507,16 +1554,19 @@
         <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1533,16 +1583,19 @@
         <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1559,16 +1612,19 @@
         <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1585,16 +1641,19 @@
         <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1611,16 +1670,19 @@
         <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>79</v>
+        <v>306</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1633,8 +1695,23 @@
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1647,8 +1724,11 @@
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1661,8 +1741,11 @@
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1675,8 +1758,11 @@
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1689,8 +1775,11 @@
       <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1703,8 +1792,11 @@
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1717,8 +1809,11 @@
       <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -1731,8 +1826,11 @@
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -1745,8 +1843,11 @@
       <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -1759,8 +1860,11 @@
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -1773,8 +1877,11 @@
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1787,8 +1894,11 @@
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1801,8 +1911,11 @@
       <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -1815,8 +1928,11 @@
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -1829,8 +1945,11 @@
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -1843,8 +1962,11 @@
       <c r="D25" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>4</v>
       </c>
@@ -1857,8 +1979,11 @@
       <c r="D26" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -1871,8 +1996,11 @@
       <c r="D27" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1885,8 +2013,11 @@
       <c r="D28" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>4</v>
       </c>
@@ -1899,8 +2030,11 @@
       <c r="D29" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>4</v>
       </c>
@@ -1913,8 +2047,11 @@
       <c r="D30" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -1927,8 +2064,11 @@
       <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
@@ -1941,6 +2081,9 @@
       <c r="D32" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J32">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -1959,16 +2102,19 @@
         <v>28</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="I33" t="s">
-        <v>300</v>
+        <v>292</v>
+      </c>
+      <c r="J33">
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -1988,13 +2134,16 @@
         <v>28</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="J34">
+        <v>32</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
@@ -2017,13 +2166,16 @@
         <v>28</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
+      </c>
+      <c r="J35">
+        <v>33</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -2046,13 +2198,16 @@
         <v>28</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
+      </c>
+      <c r="J36">
+        <v>34</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2076,13 +2231,16 @@
         <v>28</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="J37">
+        <v>35</v>
       </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -2106,13 +2264,16 @@
         <v>28</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="J38">
+        <v>36</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -2135,13 +2296,16 @@
         <v>28</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
+      </c>
+      <c r="J39">
+        <v>37</v>
       </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
@@ -2164,13 +2328,16 @@
         <v>28</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="J40">
+        <v>38</v>
       </c>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -2194,13 +2361,16 @@
         <v>28</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="J41">
+        <v>39</v>
       </c>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
@@ -2224,13 +2394,16 @@
         <v>28</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="J42">
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -2250,13 +2423,16 @@
         <v>28</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="J43">
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -2276,13 +2452,16 @@
         <v>28</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="J44">
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -2302,13 +2481,16 @@
         <v>28</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="J45">
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -2328,13 +2510,16 @@
         <v>28</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="J46">
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -2354,13 +2539,16 @@
         <v>28</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="J47">
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -2380,16 +2568,19 @@
         <v>28</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>4</v>
       </c>
@@ -2406,16 +2597,19 @@
         <v>28</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="J49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>4</v>
       </c>
@@ -2432,16 +2626,19 @@
         <v>28</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="J50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>4</v>
       </c>
@@ -2458,16 +2655,19 @@
         <v>28</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>4</v>
       </c>
@@ -2484,16 +2684,19 @@
         <v>28</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="J52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>4</v>
       </c>
@@ -2510,16 +2713,19 @@
         <v>28</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="J53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>4</v>
       </c>
@@ -2536,16 +2742,19 @@
         <v>28</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="J54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>4</v>
       </c>
@@ -2562,16 +2771,19 @@
         <v>28</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="J55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>4</v>
       </c>
@@ -2588,16 +2800,19 @@
         <v>28</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="J56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>4</v>
       </c>
@@ -2614,16 +2829,19 @@
         <v>28</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="J57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2640,16 +2858,19 @@
         <v>28</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="J58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>4</v>
       </c>
@@ -2666,16 +2887,19 @@
         <v>28</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="J59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>4</v>
       </c>
@@ -2692,16 +2916,19 @@
         <v>28</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="J60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>4</v>
       </c>
@@ -2718,16 +2945,19 @@
         <v>28</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="J61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>4</v>
       </c>
@@ -2744,16 +2974,19 @@
         <v>28</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="J62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>4</v>
       </c>
@@ -2770,16 +3003,19 @@
         <v>28</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="J63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>4</v>
       </c>
@@ -2796,16 +3032,19 @@
         <v>28</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="J64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2822,16 +3061,22 @@
         <v>28</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="J65">
+        <v>63</v>
+      </c>
+      <c r="K65" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>4</v>
       </c>
@@ -2848,7 +3093,7 @@
         <v>28</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>35</v>
@@ -2856,8 +3101,11 @@
       <c r="H66" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
@@ -2874,7 +3122,7 @@
         <v>28</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>33</v>
@@ -2882,8 +3130,11 @@
       <c r="H67" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>4</v>
       </c>
@@ -2900,7 +3151,7 @@
         <v>29</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>34</v>
@@ -2908,8 +3159,11 @@
       <c r="H68" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>4</v>
       </c>
@@ -2926,7 +3180,7 @@
         <v>29</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>36</v>
@@ -2934,8 +3188,11 @@
       <c r="H69" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>4</v>
       </c>
@@ -2952,16 +3209,19 @@
         <v>28</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="J70">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>4</v>
       </c>
@@ -2978,16 +3238,19 @@
         <v>28</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="J71">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>4</v>
       </c>
@@ -2998,22 +3261,25 @@
         <v>16</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H72" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="J72">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>4</v>
       </c>
@@ -3024,22 +3290,25 @@
         <v>17</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H73" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="J73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>4</v>
       </c>
@@ -3050,22 +3319,25 @@
         <v>18</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H74" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="J74">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>4</v>
       </c>
@@ -3076,22 +3348,25 @@
         <v>19</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H75" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="J75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>4</v>
       </c>
@@ -3102,22 +3377,25 @@
         <v>20</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="J76">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -3128,22 +3406,25 @@
         <v>21</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="J77">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>4</v>
       </c>
@@ -3160,19 +3441,22 @@
         <v>28</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G78" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H78" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="J78">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
@@ -3189,16 +3473,19 @@
         <v>28</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G79" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H79" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="J79">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>4</v>
       </c>
@@ -3215,16 +3502,19 @@
         <v>28</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G80" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H80" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="J80">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
@@ -3241,16 +3531,19 @@
         <v>28</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G81" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H81" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="J81">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>4</v>
       </c>
@@ -3267,16 +3560,19 @@
         <v>28</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G82" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H82" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="J82">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>4</v>
       </c>
@@ -3293,16 +3589,19 @@
         <v>28</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G83" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H83" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="J83">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>4</v>
       </c>
@@ -3319,16 +3618,19 @@
         <v>28</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G84" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H84" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="J84">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>4</v>
       </c>
@@ -3345,16 +3647,19 @@
         <v>28</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G85" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H85" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J85">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>4</v>
       </c>
@@ -3365,22 +3670,25 @@
         <v>14</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G86" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H86" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="J86">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>4</v>
       </c>
@@ -3391,22 +3699,25 @@
         <v>15</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G87" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H87" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+      <c r="J87">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>4</v>
       </c>
@@ -3417,22 +3728,25 @@
         <v>16</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G88" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H88" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="J88">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>4</v>
       </c>
@@ -3443,22 +3757,25 @@
         <v>17</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G89" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H89" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="J89">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>4</v>
       </c>
@@ -3469,22 +3786,25 @@
         <v>18</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G90" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H90" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="J90">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>4</v>
       </c>
@@ -3495,22 +3815,25 @@
         <v>19</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G91" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H91" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="J91">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>4</v>
       </c>
@@ -3521,22 +3844,25 @@
         <v>20</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G92" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H92" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="J92">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>4</v>
       </c>
@@ -3547,22 +3873,28 @@
         <v>21</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F93" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G93" t="s">
+        <v>245</v>
+      </c>
+      <c r="H93" t="s">
+        <v>253</v>
+      </c>
+      <c r="J93">
+        <v>95</v>
+      </c>
+      <c r="K93" t="s">
         <v>295</v>
       </c>
-      <c r="G93" t="s">
-        <v>248</v>
-      </c>
-      <c r="H93" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>4</v>
       </c>
@@ -3579,16 +3911,19 @@
         <v>28</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="J94">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>4</v>
       </c>
@@ -3605,16 +3940,19 @@
         <v>28</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>63</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="J95">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>4</v>
       </c>
@@ -3622,23 +3960,26 @@
         <v>10</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G96" s="1" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="J96">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>4</v>
       </c>
@@ -3646,23 +3987,26 @@
         <v>11</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G97" s="1" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="J97">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>4</v>
       </c>
@@ -3671,8 +4015,11 @@
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>4</v>
       </c>
@@ -3681,8 +4028,11 @@
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>4</v>
       </c>
@@ -3691,8 +4041,11 @@
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>4</v>
       </c>
@@ -3701,8 +4054,11 @@
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>4</v>
       </c>
@@ -3711,8 +4067,11 @@
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>4</v>
       </c>
@@ -3721,8 +4080,11 @@
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>4</v>
       </c>
@@ -3731,8 +4093,11 @@
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>4</v>
       </c>
@@ -3741,8 +4106,11 @@
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>4</v>
       </c>
@@ -3751,8 +4119,11 @@
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>4</v>
       </c>
@@ -3761,8 +4132,14 @@
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107">
+        <v>111</v>
+      </c>
+      <c r="K107">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>5</v>
       </c>
@@ -3777,24 +4154,27 @@
         <v>28</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G108" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H108" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>22</v>
@@ -3803,24 +4183,27 @@
         <v>28</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="J109">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>22</v>
@@ -3829,16 +4212,19 @@
         <v>28</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="J110">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>10</v>
       </c>
@@ -3855,19 +4241,22 @@
         <v>28</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G111" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H111" t="s">
+        <v>219</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I111" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" s="4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>10</v>
       </c>
@@ -3884,16 +4273,17 @@
         <v>28</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G112" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H112" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="J112" s="4"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>10</v>
       </c>
@@ -3910,16 +4300,17 @@
         <v>28</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G113" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H113" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="J113" s="4"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>10</v>
       </c>
@@ -3936,16 +4327,17 @@
         <v>28</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G114" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H114" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="J114" s="4"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>10</v>
       </c>
@@ -3962,16 +4354,17 @@
         <v>28</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G115" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H115" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="J115" s="4"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>10</v>
       </c>
@@ -3988,16 +4381,17 @@
         <v>28</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G116" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H116" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="J116" s="4"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>10</v>
       </c>
@@ -4014,16 +4408,17 @@
         <v>28</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G117" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H117" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="J117" s="4"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>10</v>
       </c>
@@ -4040,16 +4435,17 @@
         <v>28</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G118" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H118" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="J118" s="4"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>10</v>
       </c>
@@ -4066,19 +4462,20 @@
         <v>28</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G119" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H119" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="J119" s="4"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>10</v>
       </c>
@@ -4095,16 +4492,17 @@
         <v>28</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G120" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H120" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="J120" s="4"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>10</v>
       </c>
@@ -4121,16 +4519,17 @@
         <v>28</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G121" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H121" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="J121" s="4"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>10</v>
       </c>
@@ -4147,16 +4546,17 @@
         <v>28</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G122" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H122" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="J122" s="4"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>10</v>
       </c>
@@ -4173,19 +4573,20 @@
         <v>28</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G123" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H123" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="J123" s="4"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>10</v>
       </c>
@@ -4202,19 +4603,20 @@
         <v>28</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G124" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H124" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="J124" s="4"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>10</v>
       </c>
@@ -4231,19 +4633,20 @@
         <v>28</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G125" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H125" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="J125" s="4"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>10</v>
       </c>
@@ -4260,34 +4663,44 @@
         <v>28</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G126" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H126" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+      <c r="J126" s="4"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J128">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J129">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>14</v>
       </c>
@@ -4295,23 +4708,26 @@
         <v>22</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F130" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G130" s="1" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="J130">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>15</v>
       </c>
@@ -4319,104 +4735,126 @@
         <v>22</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F131" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F131" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G131" s="1" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="J131">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>160</v>
+        <v>98</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F132" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F132" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G132" s="1" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="J132">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>160</v>
+        <v>98</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="D133" s="3"/>
       <c r="E133" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F133" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F133" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G133" s="1" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+      <c r="J133">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J134">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J135">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J136">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
+      <c r="J137">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="J111:J126"/>
     <mergeCell ref="C96:D96"/>
     <mergeCell ref="C97:D97"/>
     <mergeCell ref="C108:D108"/>
@@ -4426,22 +4864,27 @@
     <mergeCell ref="C131:D131"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I78 I119 E1:F9 I123:I124 E12:F99 G111:G126 E102:F126 E140:F1048576 E130:F137">
+  <conditionalFormatting sqref="I78 I119 I123:I124 E12:F99 G111:G126 E102:F126 E140:F1048576 E130:F137 E1:F8 E10:F10">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I111 I78">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I111 I78">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>"Yes"</formula>
+  <conditionalFormatting sqref="E140:E1048576 E130:E137 E1:E126">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Maybe"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E126 E140:E1048576 E130:E137">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Maybe"</formula>
+  <conditionalFormatting sqref="E9:F9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4454,10 +4897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB57A61-88B1-44E8-9440-A35185661196}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4467,181 +4910,232 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -4652,13 +5146,16 @@
       <c r="E18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -4669,13 +5166,16 @@
       <c r="E19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -4686,13 +5186,16 @@
       <c r="E20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -4703,8 +5206,11 @@
       <c r="E21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -4714,8 +5220,11 @@
       <c r="C22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -4726,13 +5235,16 @@
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="F23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -4742,8 +5254,11 @@
       <c r="C24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -4753,53 +5268,80 @@
       <c r="C25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
+      <c r="F33">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4826,16 +5368,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4846,10 +5388,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,10 +5402,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4874,10 +5416,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4888,10 +5430,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4902,10 +5444,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4916,10 +5458,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4930,10 +5472,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4944,10 +5486,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4958,10 +5500,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4972,10 +5514,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,10 +5528,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5000,10 +5542,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5014,10 +5556,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5028,10 +5570,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5042,10 +5584,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5056,10 +5598,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>